<commit_message>
wierd register reading error
</commit_message>
<xml_diff>
--- a/remote/comm/mapping.xlsx
+++ b/remote/comm/mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asathuluri\Desktop\NewFolder\Pad_printing_machine\Complete_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asathuluri\Desktop\NewFolder\Pad_printing_machine\Complete_system\remote\remote\comm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15975" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="115">
   <si>
     <t>Modbus Address</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Address in PLC</t>
   </si>
   <si>
-    <t>Label-9</t>
-  </si>
-  <si>
     <t>Label-10</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Pi- System Error</t>
   </si>
   <si>
-    <t>*Reserved for Pi*</t>
-  </si>
-  <si>
     <t>*Reserved for PLC*</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>Reserved in PLC for future use</t>
   </si>
   <si>
-    <t>Reserved in Pi for future use</t>
-  </si>
-  <si>
     <t>The signal will be True and indicate when Pi board is in Healthy condition, else False</t>
   </si>
   <si>
@@ -170,12 +161,6 @@
     <t>This signal will be True when there will be any error in Pi system or Pi-Camera interfacing</t>
   </si>
   <si>
-    <t>*Note-</t>
-  </si>
-  <si>
-    <t>Address in Pi represented as Labels will be actual Tags defined in Raspberry Pi</t>
-  </si>
-  <si>
     <t>Model Selection-1</t>
   </si>
   <si>
@@ -269,9 +254,6 @@
     <t>To identify Module-4, this signal will be True, else False</t>
   </si>
   <si>
-    <t>Label-61</t>
-  </si>
-  <si>
     <t>reg_plc_health</t>
   </si>
   <si>
@@ -317,22 +299,76 @@
     <t>reg_pi_ori_nok</t>
   </si>
   <si>
-    <t>reg_model_1</t>
-  </si>
-  <si>
-    <t>reg_model_2</t>
-  </si>
-  <si>
-    <t>reg_model_3</t>
-  </si>
-  <si>
-    <t>reg_model_4</t>
-  </si>
-  <si>
     <t>Address type</t>
   </si>
   <si>
     <t>Register_tag</t>
+  </si>
+  <si>
+    <t>reg_plc_model</t>
+  </si>
+  <si>
+    <t>PLC-HMI-Selected model</t>
+  </si>
+  <si>
+    <t>Model selected by operator for the current cycle</t>
+  </si>
+  <si>
+    <t>reg_pi_model_1</t>
+  </si>
+  <si>
+    <t>reg_pi_model_4</t>
+  </si>
+  <si>
+    <t>reg_pi_model_3</t>
+  </si>
+  <si>
+    <t>reg_pi_model_2</t>
+  </si>
+  <si>
+    <t>reg_pi_model_nok</t>
+  </si>
+  <si>
+    <t>Model identified vs model selected nok</t>
+  </si>
+  <si>
+    <t>D62</t>
+  </si>
+  <si>
+    <t>reg_pi_model_ok</t>
+  </si>
+  <si>
+    <t>Model identified vs model selected ok</t>
+  </si>
+  <si>
+    <t>Compare between selected and identified models, ok signal</t>
+  </si>
+  <si>
+    <t>Compare between selected and identified models, nok signal</t>
+  </si>
+  <si>
+    <t>D63</t>
+  </si>
+  <si>
+    <t>reg_pi_unknown_error</t>
+  </si>
+  <si>
+    <t>To handle any other unknown errors</t>
+  </si>
+  <si>
+    <t>Default handler to denote any read/write or connection or camera or pi power issues</t>
+  </si>
+  <si>
+    <t>D64</t>
+  </si>
+  <si>
+    <t>reg_pi_last_loop</t>
+  </si>
+  <si>
+    <t>Diagnostics</t>
+  </si>
+  <si>
+    <t>Saves last entered loop before failing</t>
   </si>
 </sst>
 </file>
@@ -362,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,14 +417,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -418,19 +448,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -468,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -480,16 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -499,16 +506,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -791,25 +804,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -818,12 +831,12 @@
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -838,13 +851,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -858,13 +871,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -878,13 +891,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -898,13 +911,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -918,13 +931,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -938,13 +951,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -958,13 +971,13 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -978,13 +991,13 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -998,13 +1011,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>94</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,13 +1031,13 @@
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,16 +1048,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,16 +1068,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,16 +1088,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,16 +1108,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,33 +1128,33 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1151,16 +1164,16 @@
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1171,16 +1184,16 @@
         <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1191,16 +1204,16 @@
         <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1210,17 +1223,17 @@
       <c r="B22" s="2">
         <v>53</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>58</v>
+      <c r="C22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1230,17 +1243,17 @@
       <c r="B23" s="2">
         <v>54</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>59</v>
+      <c r="C23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1251,16 +1264,16 @@
         <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1271,16 +1284,16 @@
         <v>56</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,16 +1304,16 @@
         <v>57</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>77</v>
+        <v>45</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,16 +1324,16 @@
         <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>78</v>
+        <v>46</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1331,16 +1344,16 @@
         <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1351,19 +1364,19 @@
         <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1371,24 +1384,76 @@
         <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>49</v>
+        <v>100</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
+        <v>62</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2">
+        <v>64</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mp issues in win, moving to linux
</commit_message>
<xml_diff>
--- a/remote/comm/mapping.xlsx
+++ b/remote/comm/mapping.xlsx
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>